<commit_message>
started updates for journal article push
</commit_message>
<xml_diff>
--- a/GroupPolarizationStatmod/data/CaseStudiesMinimal.xlsx
+++ b/GroupPolarizationStatmod/data/CaseStudiesMinimal.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mt/workspace/gp-statmod/GroupPolarizationStatmod/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mt/workspace/GroupPolarization/statmod/GroupPolarizationStatmod/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D483B8FA-C722-4E45-BEDF-2CCF1C3E9083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA351DDD-3396-E74E-BBC7-BDE9D4821061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40800" yWindow="6180" windowWidth="19200" windowHeight="21600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21600" yWindow="8020" windowWidth="21600" windowHeight="19200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FalseDiscoveryRates" sheetId="11" r:id="rId1"/>
-    <sheet name="CaseStudiesMinimal" sheetId="1" r:id="rId2"/>
-    <sheet name="ToConvert" sheetId="5" r:id="rId3"/>
-    <sheet name="Notes" sheetId="3" r:id="rId4"/>
-    <sheet name="Unique Articles" sheetId="2" r:id="rId5"/>
-    <sheet name="Notes on studies not in table" sheetId="4" r:id="rId6"/>
+    <sheet name="Articles" sheetId="12" r:id="rId2"/>
+    <sheet name="ArticleStudiesMinimal" sheetId="1" r:id="rId3"/>
+    <sheet name="ToConvert" sheetId="5" r:id="rId4"/>
+    <sheet name="Notes" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="26" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,30 +37,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="150">
   <si>
     <t>CaseStudyTag</t>
   </si>
@@ -401,19 +378,10 @@
     <t>H</t>
   </si>
   <si>
-    <t>Goetals1979</t>
-  </si>
-  <si>
-    <t>Goetals and Zanna do not even report the actual shift, just that the shifts were significant. HOLY FUCKING SHIT</t>
-  </si>
-  <si>
     <t>HillclimbSuccessThreshold</t>
   </si>
   <si>
     <t>HillclimbStepSize</t>
-  </si>
-  <si>
-    <t>HypothesizedLatentMean</t>
   </si>
   <si>
     <t>The solutions here tend to have a large pre SD for which no cases were observed in Boulder, but it is still plausible that a different group could have the sorts of statistics we found. The histograms do not disambiguate actually, because they are over all topics. Probably this is less plausible than other cases, but plausible nonetheless. Take example of California, which defeated an Affirmative Action measure. It is totally plausible that many liberals have strong views against Affirmative Action, at least 1 in 5 in some groups.</t>
@@ -542,33 +510,9 @@
     <t>This shift is not claimed to be significant, ignoring this condition.</t>
   </si>
   <si>
-    <t>Stoner1968 (Influence of widely held values JESP</t>
-  </si>
-  <si>
-    <t>McGarty, Turner, ea, GP as conformity to prototypical</t>
-  </si>
-  <si>
-    <t>Maybe another early one around Stoner time, a Pruitt paper?</t>
-  </si>
-  <si>
-    <t>Another B&amp;V or two</t>
-  </si>
-  <si>
-    <t>Another Myers</t>
-  </si>
-  <si>
     <t xml:space="preserve">This is a case where only the shift is reported. I picked two numbers I thought would work. </t>
   </si>
   <si>
-    <t xml:space="preserve">FDR = </t>
-  </si>
-  <si>
-    <t>Plausibly False Positives:</t>
-  </si>
-  <si>
-    <t>Total Reported Positives:</t>
-  </si>
-  <si>
     <t>Row Labels</t>
   </si>
   <si>
@@ -587,12 +531,6 @@
     <t>FalseDiscoveryRate</t>
   </si>
   <si>
-    <t>Wallach &amp; Kogan 1965</t>
-  </si>
-  <si>
-    <t>SEE ISENBERG REVIEW FOR SEVERAL MORE</t>
-  </si>
-  <si>
     <t>DeGaulle-Judgements-Favorable</t>
   </si>
   <si>
@@ -603,6 +541,87 @@
   </si>
   <si>
     <t xml:space="preserve">Total: </t>
+  </si>
+  <si>
+    <t>StudyTag</t>
+  </si>
+  <si>
+    <t>LatentMean</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>latPreSD</t>
+  </si>
+  <si>
+    <t>latPostSD</t>
+  </si>
+  <si>
+    <t>Authors</t>
+  </si>
+  <si>
+    <t>Abrams, Wetherell, Cochrane, Hogg, and Turner</t>
+  </si>
+  <si>
+    <t>Burnstein and Vinokur</t>
+  </si>
+  <si>
+    <t>Friedkin</t>
+  </si>
+  <si>
+    <t>Hogg, Turner, and Davidson</t>
+  </si>
+  <si>
+    <t>Krizan and Baron</t>
+  </si>
+  <si>
+    <t>Moscovici and Zavalloni</t>
+  </si>
+  <si>
+    <t>Myers</t>
+  </si>
+  <si>
+    <t>Myers and Bishop</t>
+  </si>
+  <si>
+    <t>Schkade, Sunstein, and Hastie</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Journal</t>
+  </si>
+  <si>
+    <t>British Journal of Social Psychology</t>
+  </si>
+  <si>
+    <t>Journal of Experimental Social Psychology</t>
+  </si>
+  <si>
+    <t>American Sociological Review</t>
+  </si>
+  <si>
+    <t>Basic and Applied Social Psychology</t>
+  </si>
+  <si>
+    <t>European Journal of Social Psychology</t>
+  </si>
+  <si>
+    <t>Journal of Personality and Social Psychology</t>
+  </si>
+  <si>
+    <t>Human Relations</t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>Critical Review</t>
+  </si>
+  <si>
+    <t>ArticleTag</t>
   </si>
 </sst>
 </file>
@@ -1124,7 +1143,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1161,12 +1180,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1183,6 +1196,24 @@
     <xf numFmtId="2" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1274,7 +1305,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Matthew Turner" refreshedDate="44333.493882407405" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="60" xr:uid="{D02B37FA-6238-8D48-886C-C43B030BE6DB}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:N61" sheet="CaseStudiesMinimal"/>
+    <worksheetSource ref="A1:P61" sheet="ArticleStudiesMinimal"/>
   </cacheSource>
   <cacheFields count="14">
     <cacheField name="Article" numFmtId="0">
@@ -2306,7 +2337,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2A55F5B7-C5FC-0D4E-AD02-78CC73678C7D}" name="PivotTable6" cacheId="26" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2A55F5B7-C5FC-0D4E-AD02-78CC73678C7D}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField axis="axisRow" showAll="0">
@@ -2733,7 +2764,7 @@
     <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" style="27" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" style="25" customWidth="1"/>
     <col min="5" max="5" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.1640625" bestFit="1" customWidth="1"/>
@@ -2747,180 +2778,180 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>127</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>129</v>
+      <c r="A3" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="23">
         <v>10</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="23">
         <v>10</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="25">
         <f>B4 / C4</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="23">
         <v>5</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="23">
         <v>5</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="25">
         <f t="shared" ref="D5:D13" si="0">B5 / C5</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="25">
-        <v>1</v>
-      </c>
-      <c r="C6" s="25">
-        <v>1</v>
-      </c>
-      <c r="D6" s="27">
+      <c r="B6" s="23">
+        <v>1</v>
+      </c>
+      <c r="C6" s="23">
+        <v>1</v>
+      </c>
+      <c r="D6" s="25">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="23">
         <v>8</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="23">
         <v>8</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="25">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="23">
         <v>8</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="23">
         <v>9</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="25">
         <f t="shared" si="0"/>
         <v>0.88888888888888884</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="23">
         <v>10</v>
       </c>
-      <c r="C9" s="25">
+      <c r="C9" s="23">
         <v>10</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="25">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="23">
         <v>4</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="23">
         <v>4</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="25">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="23">
         <v>2</v>
       </c>
-      <c r="C11" s="25">
+      <c r="C11" s="23">
         <v>3</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="25">
         <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="23">
         <v>2</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="23">
         <v>4</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="25">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13" s="23">
         <v>5</v>
       </c>
-      <c r="C13" s="25">
+      <c r="C13" s="23">
         <v>6</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="25">
         <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="B14" s="29">
+      <c r="A14" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="27">
         <v>55</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="27">
         <v>60</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="28">
         <f>B14 / C14</f>
         <v>0.91666666666666663</v>
       </c>
@@ -2931,2040 +2962,2304 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9875D550-7A6A-DB4D-9876-AA76AE1515D1}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.5" style="35" customWidth="1"/>
+    <col min="2" max="2" width="40.1640625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="35" customWidth="1"/>
+    <col min="4" max="4" width="40.5" style="35" customWidth="1"/>
+    <col min="5" max="5" width="47.1640625" style="36" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="35"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="33" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="35">
+        <v>1990</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="35">
+        <v>1973</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="35">
+        <v>1975</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="35">
+        <v>1999</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="35">
+        <v>1990</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="35">
+        <v>2007</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="35">
+        <v>1969</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="35">
+        <v>1975</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" s="35">
+        <v>1970</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" s="35">
+        <v>2010</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N71"/>
+  <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G63" sqref="G63:H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.5" customWidth="1"/>
     <col min="2" max="2" width="32.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" customWidth="1"/>
-    <col min="9" max="9" width="25.1640625" customWidth="1"/>
-    <col min="10" max="10" width="16.1640625" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" customWidth="1"/>
-    <col min="12" max="12" width="18" customWidth="1"/>
-    <col min="13" max="13" width="15.1640625" customWidth="1"/>
-    <col min="14" max="14" width="43.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" customWidth="1"/>
+    <col min="11" max="11" width="25.1640625" customWidth="1"/>
+    <col min="12" max="12" width="16.1640625" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" customWidth="1"/>
+    <col min="14" max="14" width="18" customWidth="1"/>
+    <col min="15" max="15" width="15.1640625" customWidth="1"/>
+    <col min="16" max="16" width="43.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>125</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="I1" s="3" t="s">
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9">
         <v>5.81</v>
       </c>
-      <c r="D2" s="9">
+      <c r="F2" s="9">
         <v>6.38</v>
       </c>
-      <c r="E2" s="9">
-        <f>D2 - C2</f>
+      <c r="G2" s="9">
+        <f>F2 - E2</f>
         <v>0.57000000000000028</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="9">
+      <c r="I2" s="9">
         <v>6.2</v>
       </c>
-      <c r="H2" s="9">
+      <c r="J2" s="9">
         <v>0.05</v>
       </c>
-      <c r="I2" s="9">
+      <c r="K2" s="9">
         <v>0.05</v>
       </c>
-      <c r="J2" s="9">
-        <v>1</v>
-      </c>
-      <c r="K2" s="9">
+      <c r="L2" s="9">
+        <v>1</v>
+      </c>
+      <c r="M2" s="9">
         <v>10</v>
       </c>
-      <c r="L2" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M2" s="9">
-        <f>IF(L2, 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N2" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2" s="9">
+        <f>IF(N2, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9">
         <v>2.84</v>
       </c>
-      <c r="D3" s="9">
+      <c r="F3" s="9">
         <v>1.61</v>
       </c>
-      <c r="E3" s="9">
-        <f t="shared" ref="E3:E14" si="0">D3 - C3</f>
+      <c r="G3" s="9">
+        <f t="shared" ref="G3:G14" si="0">F3 - E3</f>
         <v>-1.2299999999999998</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="H3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="9">
+      <c r="I3" s="9">
         <v>1.6</v>
       </c>
-      <c r="H3" s="9">
+      <c r="J3" s="9">
         <v>0.05</v>
       </c>
-      <c r="I3" s="18">
+      <c r="K3" s="18">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J3" s="9">
-        <v>1</v>
-      </c>
-      <c r="K3" s="9">
+      <c r="L3" s="9">
+        <v>1</v>
+      </c>
+      <c r="M3" s="9">
         <v>10</v>
       </c>
-      <c r="L3" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M3" s="9">
-        <f t="shared" ref="M3:M61" si="1">IF(L3, 1, 0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N3" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O3" s="9">
+        <f t="shared" ref="O3:O61" si="1">IF(N3, 1, 0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9">
         <v>9.2200000000000006</v>
       </c>
-      <c r="D4" s="9">
+      <c r="F4" s="9">
         <v>9.69</v>
       </c>
-      <c r="E4" s="9">
+      <c r="G4" s="9">
         <f t="shared" si="0"/>
         <v>0.46999999999999886</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="9">
+      <c r="I4" s="9">
         <v>9.6</v>
       </c>
-      <c r="H4" s="9">
+      <c r="J4" s="9">
         <v>0.05</v>
       </c>
-      <c r="I4" s="18">
+      <c r="K4" s="18">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J4" s="9">
-        <v>1</v>
-      </c>
-      <c r="K4" s="9">
+      <c r="L4" s="9">
+        <v>1</v>
+      </c>
+      <c r="M4" s="9">
         <v>10</v>
       </c>
-      <c r="L4" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M4" s="9">
+      <c r="N4" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O4" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9">
         <v>2.48</v>
       </c>
-      <c r="D5" s="9">
+      <c r="F5" s="9">
         <v>2.19</v>
       </c>
-      <c r="E5" s="9">
+      <c r="G5" s="9">
         <f t="shared" si="0"/>
         <v>-0.29000000000000004</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="9">
+      <c r="I5" s="9">
         <v>2.2000000000000002</v>
       </c>
-      <c r="H5" s="9">
+      <c r="J5" s="9">
         <v>0.05</v>
       </c>
-      <c r="I5" s="18">
+      <c r="K5" s="18">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J5" s="9">
-        <v>1</v>
-      </c>
-      <c r="K5" s="9">
+      <c r="L5" s="9">
+        <v>1</v>
+      </c>
+      <c r="M5" s="9">
         <v>10</v>
       </c>
-      <c r="L5" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M5" s="9">
+      <c r="N5" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O5" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9">
         <v>9.19</v>
       </c>
-      <c r="D6" s="9">
+      <c r="F6" s="9">
         <v>9.44</v>
       </c>
-      <c r="E6" s="9">
+      <c r="G6" s="9">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="H6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="9">
+      <c r="I6" s="9">
         <v>9.5</v>
       </c>
-      <c r="H6" s="9">
+      <c r="J6" s="9">
         <v>0.05</v>
       </c>
-      <c r="I6" s="18">
+      <c r="K6" s="18">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J6" s="9">
-        <v>1</v>
-      </c>
-      <c r="K6" s="9">
+      <c r="L6" s="9">
+        <v>1</v>
+      </c>
+      <c r="M6" s="9">
         <v>10</v>
       </c>
-      <c r="L6" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M6" s="9">
+      <c r="N6" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O6" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9">
         <v>5.13</v>
       </c>
-      <c r="D7" s="9">
+      <c r="F7" s="9">
         <v>2.97</v>
       </c>
-      <c r="E7" s="9">
+      <c r="G7" s="9">
         <f t="shared" si="0"/>
         <v>-2.1599999999999997</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>30</v>
-      </c>
       <c r="H7" s="9" t="s">
         <v>30</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J7" s="9">
-        <v>1</v>
-      </c>
-      <c r="K7" s="9">
+      <c r="J7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="9">
+        <v>1</v>
+      </c>
+      <c r="M7" s="9">
         <v>10</v>
       </c>
-      <c r="L7" s="9" t="b">
+      <c r="N7" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="M7" s="9">
+      <c r="O7" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N7" s="9" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P7" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11">
         <v>-0.61</v>
       </c>
-      <c r="D8" s="11">
+      <c r="F8" s="11">
         <v>-1.04</v>
       </c>
-      <c r="E8" s="11">
+      <c r="G8" s="11">
         <f t="shared" si="0"/>
         <v>-0.43000000000000005</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="H8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="11">
+      <c r="I8" s="11">
         <v>-1.2</v>
       </c>
-      <c r="H8" s="11">
+      <c r="J8" s="11">
         <v>0.05</v>
       </c>
-      <c r="I8" s="19">
+      <c r="K8" s="19">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J8" s="11">
+      <c r="L8" s="11">
         <v>-3</v>
       </c>
-      <c r="K8" s="11">
+      <c r="M8" s="11">
         <v>3</v>
       </c>
-      <c r="L8" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M8" s="11">
+      <c r="N8" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O8" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11">
         <v>0.9</v>
       </c>
-      <c r="D9" s="11">
+      <c r="F9" s="11">
         <v>1.19</v>
       </c>
-      <c r="E9" s="11">
+      <c r="G9" s="11">
         <f t="shared" si="0"/>
         <v>0.28999999999999992</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="H9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="11">
+      <c r="I9" s="11">
         <v>1.2</v>
       </c>
-      <c r="H9" s="11">
+      <c r="J9" s="11">
         <v>0.05</v>
       </c>
-      <c r="I9" s="19">
+      <c r="K9" s="19">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J9" s="11">
+      <c r="L9" s="11">
         <v>-3</v>
       </c>
-      <c r="K9" s="11">
+      <c r="M9" s="11">
         <v>3</v>
       </c>
-      <c r="L9" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M9" s="11">
+      <c r="N9" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O9" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="C10" s="11">
+        <v>119</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11">
         <v>5.53</v>
       </c>
-      <c r="D10" s="11">
+      <c r="F10" s="11">
         <v>5.91</v>
       </c>
-      <c r="E10" s="11">
+      <c r="G10" s="11">
         <v>0.38</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="H10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="11">
+      <c r="I10" s="11">
         <v>6</v>
       </c>
-      <c r="H10" s="11">
+      <c r="J10" s="11">
         <v>0.01</v>
       </c>
-      <c r="I10" s="19">
+      <c r="K10" s="19">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="J10" s="11">
-        <v>1</v>
-      </c>
-      <c r="K10" s="11">
+      <c r="L10" s="11">
+        <v>1</v>
+      </c>
+      <c r="M10" s="11">
         <v>7</v>
       </c>
-      <c r="L10" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M10" s="11">
-        <f t="shared" ref="M10:M11" si="2">IF(L10, 1, 0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N10" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O10" s="11">
+        <f t="shared" ref="O10:O11" si="2">IF(N10, 1, 0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="C11" s="11">
+        <v>120</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11">
         <v>2.25</v>
       </c>
-      <c r="D11" s="11">
+      <c r="F11" s="11">
         <v>1.92</v>
       </c>
-      <c r="E11" s="11">
+      <c r="G11" s="11">
         <v>-0.37</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="H11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="11">
+      <c r="I11" s="11">
         <v>1.8</v>
       </c>
-      <c r="H11" s="11">
+      <c r="J11" s="11">
         <v>0.01</v>
       </c>
-      <c r="I11" s="19">
+      <c r="K11" s="19">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="J11" s="11">
-        <v>1</v>
-      </c>
-      <c r="K11" s="11">
+      <c r="L11" s="11">
+        <v>1</v>
+      </c>
+      <c r="M11" s="11">
         <v>7</v>
       </c>
-      <c r="L11" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M11" s="11">
+      <c r="N11" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O11" s="11">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>71</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9">
         <v>2.94</v>
       </c>
-      <c r="D12" s="9">
+      <c r="F12" s="9">
         <v>3.41</v>
       </c>
-      <c r="E12" s="9">
+      <c r="G12" s="9">
         <f t="shared" si="0"/>
         <v>0.4700000000000002</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="H12" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="9">
+      <c r="I12" s="9">
         <v>3.4</v>
       </c>
-      <c r="H12" s="9">
+      <c r="J12" s="9">
         <v>0.05</v>
       </c>
-      <c r="I12" s="18">
+      <c r="K12" s="18">
         <v>0.01</v>
       </c>
-      <c r="J12" s="9">
+      <c r="L12" s="9">
         <v>-9</v>
       </c>
-      <c r="K12" s="9">
+      <c r="M12" s="9">
         <v>9</v>
       </c>
-      <c r="L12" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M12" s="9">
+      <c r="N12" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O12" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>71</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9">
         <v>1.3</v>
       </c>
-      <c r="D13" s="9">
+      <c r="F13" s="9">
         <v>0.67</v>
       </c>
-      <c r="E13" s="9">
+      <c r="G13" s="9">
         <f t="shared" si="0"/>
         <v>-0.63</v>
       </c>
-      <c r="F13" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>30</v>
-      </c>
       <c r="H13" s="9" t="s">
         <v>30</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="L13" s="9">
         <v>-9</v>
       </c>
-      <c r="K13" s="9">
+      <c r="M13" s="9">
         <v>9</v>
       </c>
-      <c r="L13" s="9" t="b">
+      <c r="N13" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="M13" s="9">
+      <c r="O13" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N13" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P13" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>71</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9">
         <v>-1.7</v>
       </c>
-      <c r="D14" s="9">
+      <c r="F14" s="9">
         <v>-3.01</v>
       </c>
-      <c r="E14" s="9">
+      <c r="G14" s="9">
         <f t="shared" si="0"/>
         <v>-1.3099999999999998</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="H14" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="9">
+      <c r="I14" s="9">
         <v>-3</v>
       </c>
-      <c r="H14" s="9">
+      <c r="J14" s="9">
         <v>0.05</v>
       </c>
-      <c r="I14" s="18">
+      <c r="K14" s="18">
         <v>1E-3</v>
       </c>
-      <c r="J14" s="9">
+      <c r="L14" s="9">
         <v>-9</v>
       </c>
-      <c r="K14" s="9">
+      <c r="M14" s="9">
         <v>9</v>
       </c>
-      <c r="L14" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M14" s="9">
+      <c r="N14" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O14" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="11">
         <f>20 * (  ToConvert!C2  / 100)</f>
         <v>9.74</v>
       </c>
-      <c r="D15" s="11">
+      <c r="F15" s="11">
         <f>20 * (  ToConvert!D2  / 100)</f>
         <v>8.82</v>
       </c>
-      <c r="E15" s="11">
+      <c r="G15" s="11">
         <f>20 * (  ToConvert!E2  / 100)</f>
         <v>1.7199999999999998</v>
       </c>
-      <c r="F15" s="11">
+      <c r="H15" s="11">
         <f>20 * (  ToConvert!F2  / 100)</f>
         <v>1.5720000000000001</v>
       </c>
-      <c r="G15" s="11">
+      <c r="I15" s="11">
         <v>8.6999999999999993</v>
       </c>
-      <c r="H15" s="11">
+      <c r="J15" s="11">
         <v>0.5</v>
       </c>
-      <c r="I15" s="11">
+      <c r="K15" s="11">
         <v>0.05</v>
       </c>
-      <c r="J15" s="11">
-        <v>1</v>
-      </c>
-      <c r="K15" s="11">
+      <c r="L15" s="11">
+        <v>1</v>
+      </c>
+      <c r="M15" s="11">
         <v>20</v>
       </c>
-      <c r="L15" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M15" s="11">
+      <c r="N15" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O15" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N15" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P15" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="11">
+      <c r="E16" s="11">
         <f>20 * (  ToConvert!C3  / 100)</f>
         <v>9.3059999999999992</v>
       </c>
-      <c r="D16" s="11">
+      <c r="F16" s="11">
         <f>20 * (  ToConvert!D3  / 100)</f>
         <v>9.16</v>
       </c>
-      <c r="E16" s="11">
+      <c r="G16" s="11">
         <f>20 * (  ToConvert!E3  / 100)</f>
         <v>1.736</v>
       </c>
-      <c r="F16" s="11">
+      <c r="H16" s="11">
         <f>20 * (  ToConvert!F3  / 100)</f>
         <v>1.8520000000000001</v>
       </c>
-      <c r="G16" s="11">
+      <c r="I16" s="11">
         <v>9.1</v>
       </c>
-      <c r="H16" s="11">
+      <c r="J16" s="11">
         <v>0.5</v>
       </c>
-      <c r="I16" s="11">
+      <c r="K16" s="11">
         <v>0.05</v>
       </c>
-      <c r="J16" s="11">
-        <v>1</v>
-      </c>
-      <c r="K16" s="11">
+      <c r="L16" s="11">
+        <v>1</v>
+      </c>
+      <c r="M16" s="11">
         <v>20</v>
       </c>
-      <c r="L16" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M16" s="11">
+      <c r="N16" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O16" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N16" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P16" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="11">
+      <c r="E17" s="11">
         <f>20 * (  ToConvert!C4  / 100)</f>
         <v>13.62</v>
       </c>
-      <c r="D17" s="11">
+      <c r="F17" s="11">
         <f>20 * (  ToConvert!D4  / 100)</f>
         <v>13.81</v>
       </c>
-      <c r="E17" s="11">
+      <c r="G17" s="11">
         <f>20 * (  ToConvert!E4  / 100)</f>
         <v>1.25</v>
       </c>
-      <c r="F17" s="11">
+      <c r="H17" s="11">
         <f>20 * (  ToConvert!F4  / 100)</f>
         <v>0.90999999999999992</v>
       </c>
-      <c r="G17" s="11">
+      <c r="I17" s="11">
         <v>13.8</v>
       </c>
-      <c r="H17" s="11">
+      <c r="J17" s="11">
         <v>0.5</v>
       </c>
-      <c r="I17" s="19">
+      <c r="K17" s="19">
         <v>1E-3</v>
       </c>
-      <c r="J17" s="11">
-        <v>1</v>
-      </c>
-      <c r="K17" s="11">
+      <c r="L17" s="11">
+        <v>1</v>
+      </c>
+      <c r="M17" s="11">
         <v>20</v>
       </c>
-      <c r="L17" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M17" s="11">
+      <c r="N17" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O17" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="11">
         <f>20 * (  ToConvert!C5  / 100)</f>
         <v>10.532</v>
       </c>
-      <c r="D18" s="11">
+      <c r="F18" s="11">
         <f>20 * (  ToConvert!D5  / 100)</f>
         <v>9.4480000000000004</v>
       </c>
-      <c r="E18" s="11">
+      <c r="G18" s="11">
         <f>20 * (  ToConvert!E5  / 100)</f>
         <v>1.6879999999999997</v>
       </c>
-      <c r="F18" s="11">
+      <c r="H18" s="11">
         <f>20 * (  ToConvert!F5  / 100)</f>
         <v>1.8920000000000001</v>
       </c>
-      <c r="G18" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>30</v>
-      </c>
       <c r="I18" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J18" s="11">
-        <v>1</v>
-      </c>
-      <c r="K18" s="11">
+      <c r="J18" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L18" s="11">
+        <v>1</v>
+      </c>
+      <c r="M18" s="11">
         <v>20</v>
       </c>
-      <c r="L18" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M18" s="11">
+      <c r="N18" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O18" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N18" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P18" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="11">
         <f>20 * (  ToConvert!C6  / 100)</f>
         <v>10.968</v>
       </c>
-      <c r="D19" s="11">
+      <c r="F19" s="11">
         <f>20 * (  ToConvert!D6  / 100)</f>
         <v>10.844000000000001</v>
       </c>
-      <c r="E19" s="11">
+      <c r="G19" s="11">
         <f>20 * (  ToConvert!E6  / 100)</f>
         <v>1.5</v>
       </c>
-      <c r="F19" s="11">
+      <c r="H19" s="11">
         <f>20 * (  ToConvert!F6  / 100)</f>
         <v>1.226</v>
       </c>
-      <c r="G19" s="11">
+      <c r="I19" s="11">
         <v>10.9</v>
       </c>
-      <c r="H19" s="11">
+      <c r="J19" s="11">
         <v>0.5</v>
       </c>
-      <c r="I19" s="11">
+      <c r="K19" s="11">
         <v>0.05</v>
       </c>
-      <c r="J19" s="11">
-        <v>1</v>
-      </c>
-      <c r="K19" s="11">
+      <c r="L19" s="11">
+        <v>1</v>
+      </c>
+      <c r="M19" s="11">
         <v>20</v>
       </c>
-      <c r="L19" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M19" s="11">
+      <c r="N19" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O19" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N19" s="11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P19" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="11">
         <f>20 * (  ToConvert!C7  / 100)</f>
         <v>14.321999999999999</v>
       </c>
-      <c r="D20" s="11">
+      <c r="F20" s="11">
         <f>20 * (  ToConvert!D7  / 100)</f>
         <v>14.831999999999999</v>
       </c>
-      <c r="E20" s="11">
+      <c r="G20" s="11">
         <f>20 * (  ToConvert!E7  / 100)</f>
         <v>1.1640000000000001</v>
       </c>
-      <c r="F20" s="11">
+      <c r="H20" s="11">
         <f>20 * (  ToConvert!F7  / 100)</f>
         <v>1.1300000000000001</v>
       </c>
-      <c r="G20" s="11">
+      <c r="I20" s="11">
         <v>14.8</v>
       </c>
-      <c r="H20" s="11">
+      <c r="J20" s="11">
         <v>0.5</v>
       </c>
-      <c r="I20" s="19">
+      <c r="K20" s="19">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J20" s="11">
-        <v>1</v>
-      </c>
-      <c r="K20" s="11">
+      <c r="L20" s="11">
+        <v>1</v>
+      </c>
+      <c r="M20" s="11">
         <v>20</v>
       </c>
-      <c r="L20" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M20" s="11">
+      <c r="N20" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O20" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="11">
         <f>20 * (  ToConvert!C8  / 100)</f>
         <v>13.952</v>
       </c>
-      <c r="D21" s="11">
+      <c r="F21" s="11">
         <f>20 * (  ToConvert!D8  / 100)</f>
         <v>14.336000000000002</v>
       </c>
-      <c r="E21" s="11">
+      <c r="G21" s="11">
         <f>20 * (  ToConvert!E8  / 100)</f>
         <v>1.3380000000000001</v>
       </c>
-      <c r="F21" s="11">
+      <c r="H21" s="11">
         <f>20 * (  ToConvert!F8  / 100)</f>
         <v>1.3900000000000001</v>
       </c>
-      <c r="G21" s="11">
+      <c r="I21" s="11">
         <v>14.3</v>
       </c>
-      <c r="H21" s="11">
+      <c r="J21" s="11">
         <v>0.5</v>
       </c>
-      <c r="I21" s="19">
+      <c r="K21" s="19">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J21" s="11">
-        <v>1</v>
-      </c>
-      <c r="K21" s="11">
+      <c r="L21" s="11">
+        <v>1</v>
+      </c>
+      <c r="M21" s="11">
         <v>20</v>
       </c>
-      <c r="L21" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M21" s="11">
+      <c r="N21" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O21" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="11">
         <f>20 * (  ToConvert!C9  / 100)</f>
         <v>10.83</v>
       </c>
-      <c r="D22" s="11">
+      <c r="F22" s="11">
         <f>20 * (  ToConvert!D9  / 100)</f>
         <v>11.013999999999999</v>
       </c>
-      <c r="E22" s="11">
+      <c r="G22" s="11">
         <f>20 * (  ToConvert!E9  / 100)</f>
         <v>1.736</v>
       </c>
-      <c r="F22" s="11">
+      <c r="H22" s="11">
         <f>20 * (  ToConvert!F9  / 100)</f>
         <v>2.1059999999999999</v>
       </c>
-      <c r="G22" s="11">
+      <c r="I22" s="11">
         <v>11</v>
       </c>
-      <c r="H22" s="11">
+      <c r="J22" s="11">
         <v>0.5</v>
       </c>
-      <c r="I22" s="19">
+      <c r="K22" s="19">
         <v>0.05</v>
       </c>
-      <c r="J22" s="11">
-        <v>1</v>
-      </c>
-      <c r="K22" s="11">
+      <c r="L22" s="11">
+        <v>1</v>
+      </c>
+      <c r="M22" s="11">
         <v>20</v>
       </c>
-      <c r="L22" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M22" s="11">
+      <c r="N22" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O22" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N22" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P22" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="9">
         <f>10 *  ToConvert!C10</f>
         <v>5.3000000000000007</v>
       </c>
-      <c r="D23" s="9">
+      <c r="F23" s="9">
         <f>10 *  ToConvert!D10</f>
         <v>5.42</v>
       </c>
-      <c r="E23" s="9">
+      <c r="G23" s="9">
         <f>10 *  ToConvert!E10</f>
         <v>0.12</v>
       </c>
-      <c r="F23" s="9">
+      <c r="H23" s="9">
         <f>10 *  ToConvert!F10</f>
         <v>2.13</v>
       </c>
-      <c r="G23" s="9">
+      <c r="I23" s="9">
         <v>5.4</v>
       </c>
-      <c r="H23" s="9">
+      <c r="J23" s="9">
         <v>0.5</v>
       </c>
-      <c r="I23" s="18">
+      <c r="K23" s="18">
         <v>0.05</v>
       </c>
-      <c r="J23" s="9">
-        <v>1</v>
-      </c>
-      <c r="K23" s="9">
+      <c r="L23" s="9">
+        <v>1</v>
+      </c>
+      <c r="M23" s="9">
         <v>10</v>
       </c>
-      <c r="L23" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M23" s="9">
+      <c r="N23" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O23" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N23" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P23" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="9">
         <f>10 *  ToConvert!C11</f>
         <v>5.6000000000000005</v>
       </c>
-      <c r="D24" s="9">
+      <c r="F24" s="9">
         <f>10 *  ToConvert!D11</f>
         <v>4.8800000000000008</v>
       </c>
-      <c r="E24" s="9">
+      <c r="G24" s="9">
         <f>10 *  ToConvert!E11</f>
         <v>-0.72</v>
       </c>
-      <c r="F24" s="9">
+      <c r="H24" s="9">
         <f>10 *  ToConvert!F11</f>
         <v>3.14</v>
       </c>
-      <c r="G24" s="9">
+      <c r="I24" s="9">
         <v>5</v>
       </c>
-      <c r="H24" s="9">
+      <c r="J24" s="9">
         <v>0.1</v>
       </c>
-      <c r="I24" s="9">
+      <c r="K24" s="9">
         <v>0.05</v>
       </c>
-      <c r="J24" s="9">
-        <v>1</v>
-      </c>
-      <c r="K24" s="9">
+      <c r="L24" s="9">
+        <v>1</v>
+      </c>
+      <c r="M24" s="9">
         <v>10</v>
       </c>
-      <c r="L24" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M24" s="9">
+      <c r="N24" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O24" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N24" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P24" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="9">
         <f>10 *  ToConvert!C12</f>
         <v>5.0999999999999996</v>
       </c>
-      <c r="D25" s="9">
+      <c r="F25" s="9">
         <f>10 *  ToConvert!D12</f>
         <v>4.1800000000000006</v>
       </c>
-      <c r="E25" s="9">
+      <c r="G25" s="9">
         <f>10 *  ToConvert!E12</f>
         <v>-0.91999999999999993</v>
       </c>
-      <c r="F25" s="9">
+      <c r="H25" s="9">
         <f>10 *  ToConvert!F12</f>
         <v>2.25</v>
       </c>
-      <c r="G25" s="9">
+      <c r="I25" s="9">
         <v>4.2</v>
       </c>
-      <c r="H25" s="9">
+      <c r="J25" s="9">
         <v>0.5</v>
       </c>
-      <c r="I25" s="18">
+      <c r="K25" s="18">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J25" s="9">
-        <v>1</v>
-      </c>
-      <c r="K25" s="9">
+      <c r="L25" s="9">
+        <v>1</v>
+      </c>
+      <c r="M25" s="9">
         <v>10</v>
       </c>
-      <c r="L25" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M25" s="9">
+      <c r="N25" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O25" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="9">
         <f>10 *  ToConvert!C13</f>
         <v>4.6999999999999993</v>
       </c>
-      <c r="D26" s="9">
+      <c r="F26" s="9">
         <f>10 *  ToConvert!D13</f>
         <v>3.3</v>
       </c>
-      <c r="E26" s="9">
+      <c r="G26" s="9">
         <f>10 *  ToConvert!E13</f>
         <v>-1.4000000000000001</v>
       </c>
-      <c r="F26" s="9">
+      <c r="H26" s="9">
         <f>10 *  ToConvert!F13</f>
         <v>2.5</v>
       </c>
-      <c r="G26" s="9">
+      <c r="I26" s="9">
         <v>3.3</v>
       </c>
-      <c r="H26" s="9">
+      <c r="J26" s="9">
         <v>0.5</v>
       </c>
-      <c r="I26" s="18">
+      <c r="K26" s="18">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J26" s="9">
-        <v>1</v>
-      </c>
-      <c r="K26" s="9">
+      <c r="L26" s="9">
+        <v>1</v>
+      </c>
+      <c r="M26" s="9">
         <v>10</v>
       </c>
-      <c r="L26" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M26" s="9">
+      <c r="N26" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O26" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="9">
         <f>10 *  ToConvert!C14</f>
         <v>5.4</v>
       </c>
-      <c r="D27" s="9">
+      <c r="F27" s="9">
         <f>10 *  ToConvert!D14</f>
         <v>5</v>
       </c>
-      <c r="E27" s="9">
+      <c r="G27" s="9">
         <f>10 *  ToConvert!E14</f>
         <v>-0.4</v>
       </c>
-      <c r="F27" s="9">
+      <c r="H27" s="9">
         <f>10 *  ToConvert!F14</f>
         <v>2.6</v>
       </c>
-      <c r="G27" s="9">
+      <c r="I27" s="9">
         <v>5.2</v>
       </c>
-      <c r="H27" s="9">
+      <c r="J27" s="9">
         <v>0.01</v>
       </c>
-      <c r="I27" s="9">
+      <c r="K27" s="9">
         <v>0.05</v>
       </c>
-      <c r="J27" s="9">
-        <v>1</v>
-      </c>
-      <c r="K27" s="9">
+      <c r="L27" s="9">
+        <v>1</v>
+      </c>
+      <c r="M27" s="9">
         <v>10</v>
       </c>
-      <c r="L27" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M27" s="9">
+      <c r="N27" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O27" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N27" s="9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P27" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="9">
         <f>10 *  ToConvert!C15</f>
         <v>5.3000000000000007</v>
       </c>
-      <c r="D28" s="9">
+      <c r="F28" s="9">
         <f>10 *  ToConvert!D15</f>
         <v>5.17</v>
       </c>
-      <c r="E28" s="9">
+      <c r="G28" s="9">
         <f>10 *  ToConvert!E15</f>
         <v>-0.13</v>
       </c>
-      <c r="F28" s="9">
+      <c r="H28" s="9">
         <f>10 *  ToConvert!F15</f>
         <v>1.6400000000000001</v>
       </c>
-      <c r="G28" s="9">
+      <c r="I28" s="9">
         <v>5.2</v>
       </c>
-      <c r="H28" s="9">
+      <c r="J28" s="9">
         <v>0.01</v>
       </c>
-      <c r="I28" s="9">
+      <c r="K28" s="9">
         <v>0.05</v>
       </c>
-      <c r="J28" s="9">
-        <v>1</v>
-      </c>
-      <c r="K28" s="9">
+      <c r="L28" s="9">
+        <v>1</v>
+      </c>
+      <c r="M28" s="9">
         <v>10</v>
       </c>
-      <c r="L28" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M28" s="9">
+      <c r="N28" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O28" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="9">
         <f>10 *  ToConvert!C16</f>
         <v>5.6000000000000005</v>
       </c>
-      <c r="D29" s="9">
+      <c r="F29" s="9">
         <f>10 *  ToConvert!D16</f>
         <v>4.6000000000000005</v>
       </c>
-      <c r="E29" s="9">
+      <c r="G29" s="9">
         <f>10 *  ToConvert!E16</f>
         <v>-1</v>
       </c>
-      <c r="F29" s="9">
+      <c r="H29" s="9">
         <f>10 *  ToConvert!F16</f>
         <v>2.84</v>
       </c>
-      <c r="G29" s="9">
+      <c r="I29" s="9">
         <v>4.5999999999999996</v>
       </c>
-      <c r="H29" s="9">
+      <c r="J29" s="9">
         <v>0.1</v>
       </c>
-      <c r="I29" s="9">
+      <c r="K29" s="9">
         <v>0.05</v>
       </c>
-      <c r="J29" s="9">
-        <v>1</v>
-      </c>
-      <c r="K29" s="9">
+      <c r="L29" s="9">
+        <v>1</v>
+      </c>
+      <c r="M29" s="9">
         <v>10</v>
       </c>
-      <c r="L29" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M29" s="9">
+      <c r="N29" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O29" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="9">
         <f>10 *  ToConvert!C17</f>
         <v>5.0999999999999996</v>
       </c>
-      <c r="D30" s="9">
+      <c r="F30" s="9">
         <f>10 *  ToConvert!D17</f>
         <v>4.87</v>
       </c>
-      <c r="E30" s="9">
+      <c r="G30" s="9">
         <f>10 *  ToConvert!E17</f>
         <v>-0.22999999999999998</v>
       </c>
-      <c r="F30" s="9">
+      <c r="H30" s="9">
         <f>10 *  ToConvert!F17</f>
         <v>1.96</v>
       </c>
-      <c r="G30" s="9">
+      <c r="I30" s="9">
         <v>4.9000000000000004</v>
       </c>
-      <c r="H30" s="9">
+      <c r="J30" s="9">
         <v>0.01</v>
       </c>
-      <c r="I30" s="9">
+      <c r="K30" s="9">
         <v>0.05</v>
       </c>
-      <c r="J30" s="9">
-        <v>1</v>
-      </c>
-      <c r="K30" s="9">
+      <c r="L30" s="9">
+        <v>1</v>
+      </c>
+      <c r="M30" s="9">
         <v>10</v>
       </c>
-      <c r="L30" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M30" s="9">
+      <c r="N30" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O30" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="9">
         <f>10 *  ToConvert!C18</f>
         <v>4.6999999999999993</v>
       </c>
-      <c r="D31" s="9">
+      <c r="F31" s="9">
         <f>10 *  ToConvert!D18</f>
         <v>3.7</v>
       </c>
-      <c r="E31" s="9">
+      <c r="G31" s="9">
         <f>10 *  ToConvert!E18</f>
         <v>-1</v>
       </c>
-      <c r="F31" s="9">
+      <c r="H31" s="9">
         <f>10 *  ToConvert!F18</f>
         <v>2.0499999999999998</v>
       </c>
-      <c r="G31" s="9">
+      <c r="I31" s="9">
         <v>3.7</v>
       </c>
-      <c r="H31" s="9">
+      <c r="J31" s="9">
         <v>0.01</v>
       </c>
-      <c r="I31" s="9">
+      <c r="K31" s="9">
         <v>0.05</v>
       </c>
-      <c r="J31" s="9">
-        <v>1</v>
-      </c>
-      <c r="K31" s="9">
+      <c r="L31" s="9">
+        <v>1</v>
+      </c>
+      <c r="M31" s="9">
         <v>10</v>
       </c>
-      <c r="L31" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M31" s="9">
+      <c r="N31" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O31" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="9">
         <f>10 *  ToConvert!C19</f>
         <v>5.4</v>
       </c>
-      <c r="D32" s="9">
+      <c r="F32" s="9">
         <f>10 *  ToConvert!D19</f>
         <v>5.4700000000000006</v>
       </c>
-      <c r="E32" s="9">
+      <c r="G32" s="9">
         <f>10 *  ToConvert!E19</f>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F32" s="9">
+      <c r="H32" s="9">
         <f>10 *  ToConvert!F19</f>
         <v>2.13</v>
       </c>
-      <c r="G32" s="9">
+      <c r="I32" s="9">
         <v>5.5</v>
       </c>
-      <c r="H32" s="9">
+      <c r="J32" s="9">
         <v>0.01</v>
       </c>
-      <c r="I32" s="9">
+      <c r="K32" s="9">
         <v>0.05</v>
       </c>
-      <c r="J32" s="9">
-        <v>1</v>
-      </c>
-      <c r="K32" s="9">
+      <c r="L32" s="9">
+        <v>1</v>
+      </c>
+      <c r="M32" s="9">
         <v>10</v>
       </c>
-      <c r="L32" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M32" s="9">
+      <c r="N32" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O32" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="12">
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="12">
         <v>0.25</v>
       </c>
-      <c r="D33" s="11">
+      <c r="F33" s="11">
         <v>-0.72</v>
       </c>
-      <c r="E33" s="11">
+      <c r="G33" s="11">
         <v>-0.97</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="H33" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G33" s="11">
+      <c r="I33" s="11">
         <v>-0.7</v>
       </c>
-      <c r="H33" s="11">
+      <c r="J33" s="11">
         <v>0.6</v>
       </c>
-      <c r="I33" s="11">
+      <c r="K33" s="11">
         <v>0.1</v>
       </c>
-      <c r="J33" s="11">
+      <c r="L33" s="11">
         <v>-4</v>
       </c>
-      <c r="K33" s="11">
+      <c r="M33" s="11">
         <v>4</v>
       </c>
-      <c r="L33" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M33" s="11">
+      <c r="N33" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O33" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N33" s="11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P33" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="11">
         <v>0.11</v>
       </c>
-      <c r="D34" s="11">
+      <c r="F34" s="11">
         <v>-0.33</v>
       </c>
-      <c r="E34" s="11">
+      <c r="G34" s="11">
         <v>-0.44</v>
       </c>
-      <c r="F34" s="11" t="s">
+      <c r="H34" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G34" s="11">
+      <c r="I34" s="11">
         <v>-0.3</v>
       </c>
-      <c r="H34" s="11">
+      <c r="J34" s="11">
         <v>0.05</v>
       </c>
-      <c r="I34" s="11">
+      <c r="K34" s="11">
         <v>0.05</v>
       </c>
-      <c r="J34" s="11">
+      <c r="L34" s="11">
         <v>-4</v>
       </c>
-      <c r="K34" s="11">
+      <c r="M34" s="11">
         <v>4</v>
       </c>
-      <c r="L34" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M34" s="11">
+      <c r="N34" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O34" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="11">
         <v>0.03</v>
       </c>
-      <c r="D35" s="11">
+      <c r="F35" s="11">
         <v>0.83</v>
-      </c>
-      <c r="E35" s="11">
-        <v>0.8</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>30</v>
       </c>
       <c r="G35" s="11">
         <v>0.8</v>
       </c>
-      <c r="H35" s="11">
+      <c r="H35" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I35" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="J35" s="11">
         <v>0.05</v>
       </c>
-      <c r="I35" s="11">
+      <c r="K35" s="11">
         <v>0.05</v>
       </c>
-      <c r="J35" s="11">
+      <c r="L35" s="11">
         <v>-4</v>
       </c>
-      <c r="K35" s="11">
+      <c r="M35" s="11">
         <v>4</v>
       </c>
-      <c r="L35" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M35" s="11">
+      <c r="N35" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O35" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="11">
         <v>0.19</v>
       </c>
-      <c r="D36" s="11">
+      <c r="F36" s="11">
         <v>-0.14000000000000001</v>
       </c>
-      <c r="E36" s="11">
+      <c r="G36" s="11">
         <v>-0.33</v>
       </c>
-      <c r="F36" s="11" t="s">
+      <c r="H36" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G36" s="11">
+      <c r="I36" s="11">
         <v>0</v>
       </c>
-      <c r="H36" s="11">
+      <c r="J36" s="11">
         <v>0.05</v>
       </c>
-      <c r="I36" s="11">
+      <c r="K36" s="11">
         <v>0.05</v>
       </c>
-      <c r="J36" s="11">
+      <c r="L36" s="11">
         <v>-4</v>
       </c>
-      <c r="K36" s="11">
+      <c r="M36" s="11">
         <v>4</v>
       </c>
-      <c r="L36" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M36" s="11">
+      <c r="N36" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O36" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N36" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P36" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B37" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="11">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D37" s="11">
+      <c r="F37" s="11">
         <v>2.5299999999999998</v>
       </c>
-      <c r="E37" s="11">
+      <c r="G37" s="11">
         <v>2.39</v>
       </c>
-      <c r="F37" s="11" t="s">
+      <c r="H37" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G37" s="11">
+      <c r="I37" s="11">
         <v>2.5</v>
       </c>
-      <c r="H37" s="11">
+      <c r="J37" s="11">
         <v>0.05</v>
       </c>
-      <c r="I37" s="11">
+      <c r="K37" s="11">
         <v>0.05</v>
       </c>
-      <c r="J37" s="11">
+      <c r="L37" s="11">
         <v>-4</v>
       </c>
-      <c r="K37" s="11">
+      <c r="M37" s="11">
         <v>4</v>
       </c>
-      <c r="L37" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M37" s="11">
+      <c r="N37" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O37" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N37" s="11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P37" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B38" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="11">
         <v>-0.06</v>
       </c>
-      <c r="D38" s="11">
+      <c r="F38" s="11">
         <v>0.08</v>
       </c>
-      <c r="E38" s="11">
+      <c r="G38" s="11">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="H38" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G38" s="11">
+      <c r="I38" s="11">
         <v>0</v>
       </c>
-      <c r="H38" s="11">
+      <c r="J38" s="11">
         <v>0.05</v>
       </c>
-      <c r="I38" s="11">
+      <c r="K38" s="11">
         <v>0.05</v>
       </c>
-      <c r="J38" s="11">
+      <c r="L38" s="11">
         <v>-4</v>
       </c>
-      <c r="K38" s="11">
+      <c r="M38" s="11">
         <v>4</v>
       </c>
-      <c r="L38" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M38" s="11">
+      <c r="N38" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O38" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N38" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P38" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B39" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="11">
         <v>0.13</v>
       </c>
-      <c r="D39" s="11">
+      <c r="F39" s="11">
         <v>2.91</v>
       </c>
-      <c r="E39" s="11">
+      <c r="G39" s="11">
         <v>2.78</v>
       </c>
-      <c r="F39" s="11" t="s">
+      <c r="H39" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G39" s="11">
+      <c r="I39" s="11">
         <v>2.9</v>
       </c>
-      <c r="H39" s="11">
+      <c r="J39" s="11">
         <v>0.05</v>
       </c>
-      <c r="I39" s="11">
+      <c r="K39" s="11">
         <v>0.05</v>
       </c>
-      <c r="J39" s="11">
+      <c r="L39" s="11">
         <v>-4</v>
       </c>
-      <c r="K39" s="11">
+      <c r="M39" s="11">
         <v>4</v>
       </c>
-      <c r="L39" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M39" s="11">
+      <c r="N39" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O39" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N39" s="11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P39" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C40" s="11">
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="11">
         <v>0.13</v>
       </c>
-      <c r="D40" s="11">
+      <c r="F40" s="11">
         <v>0.97</v>
       </c>
-      <c r="E40" s="11">
+      <c r="G40" s="11">
         <v>0.84</v>
       </c>
-      <c r="F40" s="11" t="s">
+      <c r="H40" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G40" s="11">
+      <c r="I40" s="11">
         <v>0.9</v>
       </c>
-      <c r="H40" s="11">
+      <c r="J40" s="11">
         <v>0.05</v>
       </c>
-      <c r="I40" s="11">
+      <c r="K40" s="11">
         <v>0.01</v>
       </c>
-      <c r="J40" s="11">
+      <c r="L40" s="11">
         <v>-4</v>
       </c>
-      <c r="K40" s="11">
+      <c r="M40" s="11">
         <v>4</v>
       </c>
-      <c r="L40" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M40" s="11">
+      <c r="N40" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O40" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N40" s="11" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P40" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B41" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C41" s="11">
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="11">
         <v>-0.08</v>
       </c>
-      <c r="D41" s="11">
+      <c r="F41" s="11">
         <v>-0.15</v>
       </c>
-      <c r="E41" s="11">
+      <c r="G41" s="11">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="F41" s="11" t="s">
+      <c r="H41" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="11">
+      <c r="I41" s="11">
         <v>-0.1</v>
       </c>
-      <c r="H41" s="11">
+      <c r="J41" s="11">
         <v>0.01</v>
       </c>
-      <c r="I41" s="11">
+      <c r="K41" s="11">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J41" s="11">
+      <c r="L41" s="11">
         <v>-4</v>
       </c>
-      <c r="K41" s="11">
+      <c r="M41" s="11">
         <v>4</v>
       </c>
-      <c r="L41" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M41" s="11">
+      <c r="N41" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O41" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B42" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C42" s="11">
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="11">
         <v>0.02</v>
       </c>
-      <c r="D42" s="11">
+      <c r="F42" s="11">
         <v>-0.48</v>
       </c>
-      <c r="E42" s="11">
+      <c r="G42" s="11">
         <v>-0.5</v>
       </c>
-      <c r="F42" s="11" t="s">
+      <c r="H42" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G42" s="11">
+      <c r="I42" s="11">
         <v>-0.4</v>
       </c>
-      <c r="H42" s="11">
+      <c r="J42" s="11">
         <v>0.03</v>
       </c>
-      <c r="I42" s="11">
+      <c r="K42" s="11">
         <v>0.05</v>
       </c>
-      <c r="J42" s="11">
+      <c r="L42" s="11">
         <v>-4</v>
       </c>
-      <c r="K42" s="11">
+      <c r="M42" s="11">
         <v>4</v>
       </c>
-      <c r="L42" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M42" s="11">
+      <c r="N42" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O42" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
         <v>57</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="9">
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="9">
         <v>2.14</v>
       </c>
-      <c r="D43" s="9">
-        <f>C43 + E43</f>
+      <c r="F43" s="9">
+        <f>E43 + G43</f>
         <v>2.3200000000000003</v>
       </c>
-      <c r="E43" s="9">
+      <c r="G43" s="9">
         <v>0.18</v>
       </c>
-      <c r="F43" s="9" t="s">
+      <c r="H43" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G43" s="9">
+      <c r="I43" s="9">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H43" s="9">
+      <c r="J43" s="9">
         <v>0.01</v>
       </c>
-      <c r="I43" s="9">
+      <c r="K43" s="9">
         <v>0.01</v>
       </c>
-      <c r="J43" s="9">
+      <c r="L43" s="9">
         <v>-5</v>
       </c>
-      <c r="K43" s="9">
+      <c r="M43" s="9">
         <v>5</v>
       </c>
-      <c r="L43" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M43" s="9">
+      <c r="N43" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O43" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
         <v>57</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C44" s="9">
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="9">
         <v>1.41</v>
       </c>
-      <c r="D44" s="9">
-        <f t="shared" ref="D44:D51" si="3">C44 + E44</f>
+      <c r="F44" s="9">
+        <f t="shared" ref="F44:F51" si="3">E44 + G44</f>
         <v>1.27</v>
       </c>
-      <c r="E44" s="9">
+      <c r="G44" s="9">
         <v>-0.14000000000000001</v>
       </c>
-      <c r="F44" s="9" t="s">
+      <c r="H44" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G44" s="9">
+      <c r="I44" s="9">
         <v>1.35</v>
       </c>
-      <c r="H44" s="9">
+      <c r="J44" s="9">
         <v>0.01</v>
       </c>
-      <c r="I44" s="9">
+      <c r="K44" s="9">
         <v>0.01</v>
       </c>
-      <c r="J44" s="9">
+      <c r="L44" s="9">
         <v>-5</v>
       </c>
-      <c r="K44" s="9">
+      <c r="M44" s="9">
         <v>5</v>
       </c>
-      <c r="L44" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M44" s="9">
+      <c r="N44" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O44" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
         <v>57</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C45" s="9">
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="9">
         <v>-0.86</v>
       </c>
-      <c r="D45" s="9">
+      <c r="F45" s="9">
         <f t="shared" si="3"/>
         <v>-0.86</v>
       </c>
-      <c r="E45" s="9">
+      <c r="G45" s="9">
         <v>0</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G45" s="9" t="s">
-        <v>30</v>
       </c>
       <c r="H45" s="9" t="s">
         <v>30</v>
@@ -4972,302 +5267,316 @@
       <c r="I45" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J45" s="9">
+      <c r="J45" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K45" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="L45" s="9">
         <v>-5</v>
       </c>
-      <c r="K45" s="9">
+      <c r="M45" s="9">
         <v>5</v>
       </c>
-      <c r="L45" s="9" t="b">
+      <c r="N45" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="M45" s="9">
+      <c r="O45" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
         <v>57</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="9">
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="9">
         <v>1.84</v>
       </c>
-      <c r="D46" s="9">
+      <c r="F46" s="9">
         <f t="shared" si="3"/>
         <v>2.16</v>
       </c>
-      <c r="E46" s="9">
+      <c r="G46" s="9">
         <v>0.32</v>
       </c>
-      <c r="F46" s="9" t="s">
+      <c r="H46" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G46" s="9">
+      <c r="I46" s="9">
         <v>2.1</v>
       </c>
-      <c r="H46" s="9">
+      <c r="J46" s="9">
         <v>0.01</v>
       </c>
-      <c r="I46" s="9">
+      <c r="K46" s="9">
         <v>0.01</v>
       </c>
-      <c r="J46" s="9">
+      <c r="L46" s="9">
         <v>-5</v>
       </c>
-      <c r="K46" s="9">
+      <c r="M46" s="9">
         <v>5</v>
       </c>
-      <c r="L46" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M46" s="9">
+      <c r="N46" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O46" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
         <v>57</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C47" s="9">
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="9">
         <v>-0.55000000000000004</v>
       </c>
-      <c r="D47" s="9">
+      <c r="F47" s="9">
         <f t="shared" si="3"/>
         <v>-0.44000000000000006</v>
       </c>
-      <c r="E47" s="9">
+      <c r="G47" s="9">
         <v>0.11</v>
       </c>
-      <c r="F47" s="9" t="s">
+      <c r="H47" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G47" s="9">
+      <c r="I47" s="9">
         <v>-0.4</v>
       </c>
-      <c r="H47" s="9">
+      <c r="J47" s="9">
         <v>0.01</v>
       </c>
-      <c r="I47" s="9">
+      <c r="K47" s="9">
         <v>0.05</v>
       </c>
-      <c r="J47" s="9">
+      <c r="L47" s="9">
         <v>-5</v>
       </c>
-      <c r="K47" s="9">
+      <c r="M47" s="9">
         <v>5</v>
       </c>
-      <c r="L47" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M47" s="9">
+      <c r="N47" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O47" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
         <v>57</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="9">
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="9">
         <v>-1.66</v>
       </c>
-      <c r="D48" s="9">
+      <c r="F48" s="9">
         <f t="shared" si="3"/>
         <v>-1.77</v>
       </c>
-      <c r="E48" s="9">
+      <c r="G48" s="9">
         <v>-0.11</v>
       </c>
-      <c r="F48" s="9" t="s">
+      <c r="H48" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G48" s="9">
+      <c r="I48" s="9">
         <v>-1.7</v>
       </c>
-      <c r="H48" s="9">
+      <c r="J48" s="9">
         <v>0.01</v>
       </c>
-      <c r="I48" s="9">
+      <c r="K48" s="9">
         <v>0.01</v>
       </c>
-      <c r="J48" s="9">
+      <c r="L48" s="9">
         <v>-5</v>
       </c>
-      <c r="K48" s="9">
+      <c r="M48" s="9">
         <v>5</v>
       </c>
-      <c r="L48" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M48" s="9">
+      <c r="N48" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O48" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
         <v>57</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="9">
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="9">
         <v>2.1</v>
       </c>
-      <c r="D49" s="9">
+      <c r="F49" s="9">
         <f t="shared" si="3"/>
         <v>2.5</v>
       </c>
-      <c r="E49" s="9">
+      <c r="G49" s="9">
         <v>0.4</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="H49" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G49" s="9">
+      <c r="I49" s="9">
         <v>2.5</v>
       </c>
-      <c r="H49" s="9">
+      <c r="J49" s="9">
         <v>0.01</v>
       </c>
-      <c r="I49" s="9">
+      <c r="K49" s="9">
         <v>1E-4</v>
       </c>
-      <c r="J49" s="9">
+      <c r="L49" s="9">
         <v>-5</v>
       </c>
-      <c r="K49" s="9">
+      <c r="M49" s="9">
         <v>5</v>
       </c>
-      <c r="L49" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M49" s="9">
+      <c r="N49" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O49" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
         <v>57</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C50" s="9">
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="9">
         <v>0</v>
       </c>
-      <c r="D50" s="9">
+      <c r="F50" s="9">
         <f t="shared" si="3"/>
         <v>-0.33</v>
       </c>
-      <c r="E50" s="9">
+      <c r="G50" s="9">
         <v>-0.33</v>
       </c>
-      <c r="F50" s="9" t="s">
+      <c r="H50" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G50" s="9">
+      <c r="I50" s="9">
         <v>-0.3</v>
       </c>
-      <c r="H50" s="9">
+      <c r="J50" s="9">
         <v>0.1</v>
       </c>
-      <c r="I50" s="9">
+      <c r="K50" s="9">
         <v>0.01</v>
       </c>
-      <c r="J50" s="9">
+      <c r="L50" s="9">
         <v>-5</v>
       </c>
-      <c r="K50" s="9">
+      <c r="M50" s="9">
         <v>5</v>
       </c>
-      <c r="L50" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M50" s="9">
+      <c r="N50" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O50" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
         <v>57</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C51" s="9">
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="9">
         <v>-1.93</v>
       </c>
-      <c r="D51" s="9">
+      <c r="F51" s="9">
         <f t="shared" si="3"/>
         <v>-1.74</v>
       </c>
-      <c r="E51" s="9">
+      <c r="G51" s="9">
         <v>0.19</v>
       </c>
-      <c r="F51" s="9" t="s">
+      <c r="H51" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G51" s="9">
+      <c r="I51" s="9">
         <v>-1.85</v>
       </c>
-      <c r="H51" s="9">
+      <c r="J51" s="9">
         <v>0.05</v>
       </c>
-      <c r="I51" s="9">
+      <c r="K51" s="9">
         <v>0.01</v>
       </c>
-      <c r="J51" s="9">
+      <c r="L51" s="9">
         <v>-5</v>
       </c>
-      <c r="K51" s="9">
+      <c r="M51" s="9">
         <v>5</v>
       </c>
-      <c r="L51" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M51" s="9">
+      <c r="N51" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O51" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N51" s="9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P51" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
         <v>75</v>
       </c>
       <c r="B52" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C52" s="11">
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="11">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D52" s="11">
+      <c r="F52" s="11">
         <v>3.04</v>
       </c>
-      <c r="E52" s="11">
+      <c r="G52" s="11">
         <v>-1.08</v>
-      </c>
-      <c r="F52" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G52" s="11" t="s">
-        <v>30</v>
       </c>
       <c r="H52" s="11" t="s">
         <v>30</v>
@@ -5275,464 +5584,440 @@
       <c r="I52" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J52" s="11">
+      <c r="J52" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K52" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L52" s="11">
         <v>0</v>
       </c>
-      <c r="K52" s="11">
+      <c r="M52" s="11">
         <v>10</v>
       </c>
-      <c r="L52" s="11" t="b">
+      <c r="N52" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="M52" s="9">
+      <c r="O52" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N52" s="11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P52" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
         <v>75</v>
       </c>
       <c r="B53" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C53" s="11">
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="11">
         <v>7.47</v>
       </c>
-      <c r="D53" s="11">
+      <c r="F53" s="11">
         <v>8.0500000000000007</v>
       </c>
-      <c r="E53" s="11">
+      <c r="G53" s="11">
         <v>0.59</v>
       </c>
-      <c r="F53" s="11" t="s">
+      <c r="H53" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G53">
+      <c r="I53">
         <v>8.1999999999999993</v>
       </c>
-      <c r="H53">
+      <c r="J53">
         <v>0.05</v>
       </c>
-      <c r="I53" s="20">
+      <c r="K53" s="20">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J53" s="11">
+      <c r="L53" s="11">
         <v>0</v>
       </c>
-      <c r="K53" s="11">
+      <c r="M53" s="11">
         <v>10</v>
       </c>
-      <c r="L53" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M53" s="9">
+      <c r="N53" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O53" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
         <v>75</v>
       </c>
       <c r="B54" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C54" s="11">
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="11">
         <v>-1.1100000000000001</v>
       </c>
-      <c r="D54" s="11">
+      <c r="F54" s="11">
         <v>-1.1399999999999999</v>
       </c>
-      <c r="E54" s="11">
+      <c r="G54" s="11">
         <v>-0.02</v>
       </c>
-      <c r="F54" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G54" t="s">
-        <v>30</v>
-      </c>
-      <c r="H54" t="s">
+      <c r="H54" s="11" t="s">
         <v>30</v>
       </c>
       <c r="I54" t="s">
         <v>30</v>
       </c>
-      <c r="J54" s="11">
+      <c r="J54" t="s">
+        <v>30</v>
+      </c>
+      <c r="K54" t="s">
+        <v>30</v>
+      </c>
+      <c r="L54" s="11">
         <v>-3</v>
       </c>
-      <c r="K54" s="11">
+      <c r="M54" s="11">
         <v>3</v>
       </c>
-      <c r="L54" t="b">
+      <c r="N54" t="b">
         <v>0</v>
       </c>
-      <c r="M54" s="9">
+      <c r="O54" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N54" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P54" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
         <v>75</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C55" s="11">
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="11">
         <v>0.78</v>
       </c>
-      <c r="D55" s="11">
+      <c r="F55" s="11">
         <v>1.72</v>
       </c>
-      <c r="E55" s="11">
+      <c r="G55" s="11">
         <v>0.95</v>
       </c>
-      <c r="F55" s="11" t="s">
+      <c r="H55" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G55">
+      <c r="I55">
         <v>1.7</v>
       </c>
-      <c r="H55">
+      <c r="J55">
         <v>0.02</v>
       </c>
-      <c r="I55">
+      <c r="K55">
         <v>1E-3</v>
       </c>
-      <c r="J55" s="11">
+      <c r="L55" s="11">
         <v>-3</v>
       </c>
-      <c r="K55" s="11">
+      <c r="M55" s="11">
         <v>3</v>
       </c>
-      <c r="L55" t="b">
-        <v>1</v>
-      </c>
-      <c r="M55" s="9">
+      <c r="N55" t="b">
+        <v>1</v>
+      </c>
+      <c r="O55" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
         <v>81</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C56" s="9">
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="9">
         <v>2</v>
       </c>
-      <c r="D56" s="9">
+      <c r="F56" s="9">
         <v>1.35</v>
       </c>
-      <c r="E56" s="9">
+      <c r="G56" s="9">
         <v>-0.65</v>
       </c>
-      <c r="F56" s="9" t="s">
+      <c r="H56" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G56" s="9">
+      <c r="I56" s="9">
         <v>1.3</v>
       </c>
-      <c r="H56" s="9">
+      <c r="J56" s="9">
         <v>0.1</v>
       </c>
-      <c r="I56" s="18">
+      <c r="K56" s="18">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="J56" s="9">
-        <v>1</v>
-      </c>
-      <c r="K56" s="9">
+      <c r="L56" s="9">
+        <v>1</v>
+      </c>
+      <c r="M56" s="9">
         <v>10</v>
       </c>
-      <c r="L56" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M56" s="9">
+      <c r="N56" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O56" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N56" s="9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P56" s="9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
         <v>84</v>
       </c>
       <c r="B57" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57">
         <v>4.17</v>
       </c>
-      <c r="D57">
+      <c r="F57">
         <v>3.36</v>
       </c>
-      <c r="E57" s="11">
+      <c r="G57" s="11">
         <v>-0.83</v>
       </c>
-      <c r="F57" s="11" t="s">
+      <c r="H57" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G57">
+      <c r="I57">
         <v>3.2</v>
       </c>
-      <c r="H57">
+      <c r="J57">
         <v>0.05</v>
       </c>
-      <c r="I57">
+      <c r="K57">
         <v>0.05</v>
       </c>
-      <c r="J57" s="11">
-        <v>1</v>
-      </c>
-      <c r="K57" s="11">
+      <c r="L57" s="11">
+        <v>1</v>
+      </c>
+      <c r="M57" s="11">
         <v>10</v>
       </c>
-      <c r="L57" t="b">
-        <v>1</v>
-      </c>
-      <c r="M57" s="9">
+      <c r="N57" t="b">
+        <v>1</v>
+      </c>
+      <c r="O57" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
         <v>84</v>
       </c>
       <c r="B58" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58">
         <v>5.76</v>
       </c>
-      <c r="D58">
+      <c r="F58">
         <v>5.42</v>
       </c>
-      <c r="E58" s="11">
+      <c r="G58" s="11">
         <v>-0.33</v>
       </c>
-      <c r="F58" s="11" t="s">
+      <c r="H58" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G58">
+      <c r="I58">
         <v>5.6</v>
       </c>
-      <c r="H58">
+      <c r="J58">
         <v>0.05</v>
       </c>
-      <c r="I58">
+      <c r="K58">
         <v>1E-3</v>
       </c>
-      <c r="J58" s="11">
-        <v>1</v>
-      </c>
-      <c r="K58" s="11">
+      <c r="L58" s="11">
+        <v>1</v>
+      </c>
+      <c r="M58" s="11">
         <v>10</v>
       </c>
-      <c r="L58" t="b">
-        <v>1</v>
-      </c>
-      <c r="M58" s="9">
+      <c r="N58" t="b">
+        <v>1</v>
+      </c>
+      <c r="O58" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
         <v>84</v>
       </c>
       <c r="B59" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59">
         <v>7.76</v>
       </c>
-      <c r="D59">
+      <c r="F59">
         <v>8.42</v>
       </c>
-      <c r="E59" s="11">
+      <c r="G59" s="11">
         <v>0.68</v>
       </c>
-      <c r="F59" s="11" t="s">
+      <c r="H59" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G59">
+      <c r="I59">
         <v>8.4</v>
       </c>
-      <c r="H59">
+      <c r="J59">
         <v>0.01</v>
       </c>
-      <c r="I59">
+      <c r="K59">
         <v>0.01</v>
       </c>
-      <c r="J59" s="11">
-        <v>1</v>
-      </c>
-      <c r="K59" s="11">
+      <c r="L59" s="11">
+        <v>1</v>
+      </c>
+      <c r="M59" s="11">
         <v>10</v>
       </c>
-      <c r="L59" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M59" s="9">
+      <c r="N59" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O59" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
         <v>84</v>
       </c>
       <c r="B60" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60">
         <v>8.36</v>
       </c>
-      <c r="D60">
+      <c r="F60">
         <v>8.56</v>
       </c>
-      <c r="E60" s="11">
+      <c r="G60" s="11">
         <v>0.2</v>
       </c>
-      <c r="F60" s="11" t="s">
+      <c r="H60" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G60">
+      <c r="I60">
         <v>8.5</v>
       </c>
-      <c r="H60">
+      <c r="J60">
         <v>0.01</v>
       </c>
-      <c r="I60">
+      <c r="K60">
         <v>0.01</v>
       </c>
-      <c r="J60" s="11">
-        <v>1</v>
-      </c>
-      <c r="K60" s="11">
+      <c r="L60" s="11">
+        <v>1</v>
+      </c>
+      <c r="M60" s="11">
         <v>10</v>
       </c>
-      <c r="L60" t="b">
-        <v>1</v>
-      </c>
-      <c r="M60" s="9">
+      <c r="N60" t="b">
+        <v>1</v>
+      </c>
+      <c r="O60" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
         <v>84</v>
       </c>
       <c r="B61" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61">
         <v>6.87</v>
       </c>
-      <c r="D61">
+      <c r="F61">
         <v>7.26</v>
       </c>
-      <c r="E61" s="11">
+      <c r="G61" s="11">
         <v>0.41</v>
       </c>
-      <c r="F61" s="11" t="s">
+      <c r="H61" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G61">
+      <c r="I61">
         <v>7.2</v>
       </c>
-      <c r="H61">
+      <c r="J61">
         <v>0.01</v>
       </c>
-      <c r="I61">
+      <c r="K61">
         <v>0.01</v>
       </c>
-      <c r="J61" s="11">
-        <v>1</v>
-      </c>
-      <c r="K61" s="11">
+      <c r="L61" s="11">
+        <v>1</v>
+      </c>
+      <c r="M61" s="11">
         <v>10</v>
       </c>
-      <c r="L61" t="b">
-        <v>1</v>
-      </c>
-      <c r="M61" s="9">
+      <c r="N61" t="b">
+        <v>1</v>
+      </c>
+      <c r="O61" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="E63" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="F63" s="23" cm="1">
-        <f t="array" ref="F63">SUM(IF(L2:L61 = TRUE, 1, 0)) / (62 - SUM(IF(L2:L61 = "NA", 1, 0)))</f>
-        <v>0.88709677419354838</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>116</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F66" cm="1">
-        <f t="array" ref="F66">SUM(IF(L2:L61 = TRUE, 1, 0))</f>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>118</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="F67" cm="1">
-        <f t="array" ref="F67">(64 - SUM(IF(L2:L61 = "NA", 1, 0)))</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>131</v>
-      </c>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G63" s="37"/>
+      <c r="H63" s="38"/>
+    </row>
+    <row r="66" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G66" s="5"/>
+    </row>
+    <row r="67" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G67" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
@@ -5740,7 +6025,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8172560-2780-5445-AC48-D9C066AC77F2}">
   <dimension ref="A1:F19"/>
   <sheetViews>
@@ -6153,11 +6438,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575A569A-5DEF-E74A-A53D-4EAEB49813F7}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+    <sheetView topLeftCell="B10" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -6177,7 +6462,7 @@
         <v>10</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="14" customFormat="1" ht="153" x14ac:dyDescent="0.2">
@@ -6185,7 +6470,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C2">
         <v>1008</v>
@@ -6302,8 +6587,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E13" s="34" t="s">
-        <v>135</v>
+      <c r="E13" s="32" t="s">
+        <v>122</v>
       </c>
       <c r="F13">
         <f>SUM(C2:C12)</f>
@@ -6316,156 +6601,4 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC4C913-E284-FF41-957F-B20E8BC10839}">
-  <dimension ref="A1:A18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="22.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="str" cm="1">
-        <f t="array" ref="A1:A18">_xlfn.UNIQUE(CaseStudiesMinimal!A2:A9996)</f>
-        <v>Schkade2010</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="str">
-        <v>Moscovici1969</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="str">
-        <v>Myers1970</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="str">
-        <v>Friedkin1999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="str">
-        <v>Krizan2007</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="str">
-        <v>Abrams1990</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="str">
-        <v>Hogg1990</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="str">
-        <v>Myers1975</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="str">
-        <v>Burnstein1975</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="str">
-        <v>Burnstein1973</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="str">
-        <v>Stoner1968 (Influence of widely held values JESP</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="str">
-        <v>McGarty, Turner, ea, GP as conformity to prototypical</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="str">
-        <v>Another B&amp;V or two</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="str">
-        <v>Maybe another early one around Stoner time, a Pruitt paper?</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" t="str">
-        <v>Another Myers</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="str">
-        <v>Wallach &amp; Kogan 1965</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="str">
-        <v>SEE ISENBERG REVIEW FOR SEVERAL MORE</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69900CE5-538D-0A45-870E-F27DFAA29746}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="33" style="7" customWidth="1"/>
-    <col min="2" max="2" width="97" style="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
-      <c r="B3" s="15"/>
-    </row>
-    <row r="4" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="13"/>
-      <c r="B4" s="15"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
backing up first draft case studies xl
</commit_message>
<xml_diff>
--- a/GroupPolarizationStatmod/data/CaseStudiesMinimal.xlsx
+++ b/GroupPolarizationStatmod/data/CaseStudiesMinimal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mt/workspace/GroupPolarization/statmod/GroupPolarizationStatmod/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA351DDD-3396-E74E-BBC7-BDE9D4821061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B8405B-4020-8F4D-B164-8F56D91BCE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21600" yWindow="8020" windowWidth="21600" windowHeight="19200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5520" yWindow="500" windowWidth="12160" windowHeight="19200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FalseDiscoveryRates" sheetId="11" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="149">
   <si>
     <t>CaseStudyTag</t>
   </si>
@@ -543,21 +543,9 @@
     <t xml:space="preserve">Total: </t>
   </si>
   <si>
-    <t>StudyTag</t>
-  </si>
-  <si>
     <t>LatentMean</t>
   </si>
   <si>
-    <t>Tag</t>
-  </si>
-  <si>
-    <t>latPreSD</t>
-  </si>
-  <si>
-    <t>latPostSD</t>
-  </si>
-  <si>
     <t>Authors</t>
   </si>
   <si>
@@ -622,6 +610,15 @@
   </si>
   <si>
     <t>ArticleTag</t>
+  </si>
+  <si>
+    <t>TreatmentTag</t>
+  </si>
+  <si>
+    <t>LatentSDPre</t>
+  </si>
+  <si>
+    <t>LatentSDPost</t>
   </si>
 </sst>
 </file>
@@ -2979,16 +2976,16 @@
   <sheetData>
     <row r="1" spans="1:5" s="33" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E1" s="34" t="s">
         <v>10</v>
@@ -2999,13 +2996,13 @@
         <v>22</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C2" s="35">
         <v>1990</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -3013,13 +3010,13 @@
         <v>84</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C3" s="35">
         <v>1973</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -3027,13 +3024,13 @@
         <v>81</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C4" s="35">
         <v>1975</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -3041,13 +3038,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C5" s="35">
         <v>1999</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -3055,13 +3052,13 @@
         <v>57</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C6" s="35">
         <v>1990</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -3069,13 +3066,13 @@
         <v>35</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C7" s="35">
         <v>2007</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -3083,13 +3080,13 @@
         <v>9</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C8" s="35">
         <v>1969</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -3097,13 +3094,13 @@
         <v>71</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C9" s="35">
         <v>1975</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -3111,13 +3108,13 @@
         <v>75</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C10" s="35">
         <v>1970</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -3125,13 +3122,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C11" s="35">
         <v>2010</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -3143,9 +3140,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G63" sqref="G63:H63"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3170,16 +3167,16 @@
   <sheetData>
     <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>1</v>
@@ -3194,7 +3191,7 @@
         <v>32</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>92</v>
@@ -4851,7 +4848,7 @@
         <v>30</v>
       </c>
       <c r="I36" s="11">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="J36" s="11">
         <v>0.05</v>

</xml_diff>

<commit_message>
3/10 analyzed; saving all data, means displayed correctly
</commit_message>
<xml_diff>
--- a/GroupPolarizationStatmod/data/CaseStudiesMinimal.xlsx
+++ b/GroupPolarizationStatmod/data/CaseStudiesMinimal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mt/workspace/GroupPolarization/statmod/GroupPolarizationStatmod/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B8405B-4020-8F4D-B164-8F56D91BCE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D25405-65F5-C342-A2E9-7CA92694D789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="500" windowWidth="12160" windowHeight="19200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FalseDiscoveryRates" sheetId="11" r:id="rId1"/>
@@ -3140,8 +3140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
t-test analysis done for first pass
</commit_message>
<xml_diff>
--- a/GroupPolarizationStatmod/data/CaseStudiesMinimal.xlsx
+++ b/GroupPolarizationStatmod/data/CaseStudiesMinimal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mt/workspace/GroupPolarization/statmod/GroupPolarizationStatmod/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mt/workspace/gp-statmod/GroupPolarizationStatmod/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D25405-65F5-C342-A2E9-7CA92694D789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0058EC-68E3-9C46-9BD3-E133B97D885F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25600" yWindow="3600" windowWidth="25600" windowHeight="16000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FalseDiscoveryRates" sheetId="11" r:id="rId1"/>
@@ -3140,7 +3140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+    <sheetView zoomScale="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
     </sheetView>
@@ -6439,8 +6439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575A569A-5DEF-E74A-A53D-4EAEB49813F7}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
good first draft of bar with markers for FWER, FDR
</commit_message>
<xml_diff>
--- a/GroupPolarizationStatmod/data/CaseStudiesMinimal.xlsx
+++ b/GroupPolarizationStatmod/data/CaseStudiesMinimal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mt/workspace/gp-statmod/GroupPolarizationStatmod/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5E7B0C-78F3-A84B-A2FE-7FA04FFC70D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9BA8D3-2E83-A04D-901A-B3A5BF3504B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7220" yWindow="3780" windowWidth="25600" windowHeight="16000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,6 +31,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>

</xml_diff>